<commit_message>
refactoring code with Python
</commit_message>
<xml_diff>
--- a/Mean Point guard.xlsx
+++ b/Mean Point guard.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RichardFrancais\Desktop\econometrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B87C098-35DA-4F4B-B5BD-5A399AD14048}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D30DE1-CE2C-4830-B848-A2D0C207536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21915" windowHeight="4545" xr2:uid="{1AC5DDF1-1A84-4E94-92E5-DE048250BB74}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{1AC5DDF1-1A84-4E94-92E5-DE048250BB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -247,6 +256,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,8 +288,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC4BEB-85D9-483A-B534-F4D7029A0C2B}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +677,7 @@
       <c r="F2">
         <v>33.799999999999997</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>H2/I2</f>
         <v>0.44596131968145619</v>
       </c>
@@ -696,7 +710,7 @@
       <c r="F3">
         <v>33.799999999999997</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G63" si="0">H3/I3</f>
         <v>0.43010752688172044</v>
       </c>
@@ -729,7 +743,7 @@
       <c r="F4">
         <v>34.4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0.44506726457399104</v>
       </c>
@@ -762,7 +776,7 @@
       <c r="F5">
         <v>35.700000000000003</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>0.47005649717514125</v>
       </c>
@@ -795,7 +809,7 @@
       <c r="F6">
         <v>37.5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>0.44628099173553715</v>
       </c>
@@ -828,7 +842,7 @@
       <c r="F7">
         <v>37.299999999999997</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>0.45197044334975373</v>
       </c>
@@ -861,7 +875,7 @@
       <c r="F8">
         <v>36.200000000000003</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>0.46071428571428574</v>
       </c>
@@ -894,7 +908,7 @@
       <c r="F9">
         <v>36.5</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>0.47099767981438517</v>
       </c>
@@ -927,7 +941,7 @@
       <c r="F10">
         <v>31.2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>0.4497716894977169</v>
       </c>
@@ -960,7 +974,7 @@
       <c r="F11">
         <v>31.7</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>0.43843498273878018</v>
       </c>
@@ -993,7 +1007,7 @@
       <c r="F12">
         <v>36.6</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>0.45909645909645908</v>
       </c>
@@ -1026,7 +1040,7 @@
       <c r="F13">
         <v>34.6</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>0.45714285714285713</v>
       </c>
@@ -1059,7 +1073,7 @@
       <c r="F14">
         <v>32.6</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>0.43690476190476196</v>
       </c>
@@ -1092,7 +1106,7 @@
       <c r="F15">
         <v>32.200000000000003</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>0.46390532544378704</v>
       </c>
@@ -1125,7 +1139,7 @@
       <c r="F16">
         <v>26.1</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <f t="shared" si="0"/>
         <v>0.45882352941176469</v>
       </c>
@@ -1158,7 +1172,7 @@
       <c r="F17">
         <v>27.3</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <f t="shared" si="0"/>
         <v>0.45402951191827473</v>
       </c>
@@ -1191,7 +1205,7 @@
       <c r="F18">
         <v>33.5</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>0.45146198830409356</v>
       </c>
@@ -1224,7 +1238,7 @@
       <c r="F19">
         <v>33.9</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>0.44873341375150783</v>
       </c>
@@ -1257,7 +1271,7 @@
       <c r="F20">
         <v>27.8</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f t="shared" si="0"/>
         <v>0.44071856287425148</v>
       </c>
@@ -1290,7 +1304,7 @@
       <c r="F21">
         <v>27</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <f t="shared" si="0"/>
         <v>0.48014440433212996</v>
       </c>
@@ -1323,7 +1337,7 @@
       <c r="F22">
         <v>34.5</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <f t="shared" si="0"/>
         <v>0.45328719723183386</v>
       </c>
@@ -1356,7 +1370,7 @@
       <c r="F23">
         <v>34.799999999999997</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <f t="shared" si="0"/>
         <v>0.45886442641946701</v>
       </c>
@@ -1389,7 +1403,7 @@
       <c r="F24">
         <v>32.4</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <f t="shared" si="0"/>
         <v>0.46073903002309469</v>
       </c>
@@ -1422,7 +1436,7 @@
       <c r="F25">
         <v>32.700000000000003</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="0"/>
         <v>0.4562996594778661</v>
       </c>
@@ -1455,7 +1469,7 @@
       <c r="F26">
         <v>29.7</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <f t="shared" si="0"/>
         <v>0.45093457943925236</v>
       </c>
@@ -1488,7 +1502,7 @@
       <c r="F27">
         <v>29.1</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <f t="shared" si="0"/>
         <v>0.48220436280137774</v>
       </c>
@@ -1521,7 +1535,7 @@
       <c r="F28">
         <v>24.3</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
         <v>0.44953051643192482</v>
       </c>
@@ -1554,7 +1568,7 @@
       <c r="F29">
         <v>28.4</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <f t="shared" si="0"/>
         <v>0.47113163972286376</v>
       </c>
@@ -1587,7 +1601,7 @@
       <c r="F30">
         <v>25</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <f t="shared" si="0"/>
         <v>0.44933920704845814</v>
       </c>
@@ -1620,7 +1634,7 @@
       <c r="F31">
         <v>24.4</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <f t="shared" si="0"/>
         <v>0.46754675467546752</v>
       </c>
@@ -1653,7 +1667,7 @@
       <c r="F32">
         <v>32.9</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <f t="shared" si="0"/>
         <v>0.43078626799557029</v>
       </c>
@@ -1686,7 +1700,7 @@
       <c r="F33">
         <v>34</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <f t="shared" si="0"/>
         <v>0.43977272727272732</v>
       </c>
@@ -1719,7 +1733,7 @@
       <c r="F34">
         <v>24.4</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <f t="shared" si="0"/>
         <v>0.44563918757467141</v>
       </c>
@@ -1752,7 +1766,7 @@
       <c r="F35">
         <v>26</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <f t="shared" si="0"/>
         <v>0.44043321299638993</v>
       </c>
@@ -1785,7 +1799,7 @@
       <c r="F36">
         <v>36.5</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <f t="shared" si="0"/>
         <v>0.46042363433667777</v>
       </c>
@@ -1818,7 +1832,7 @@
       <c r="F37">
         <v>36.299999999999997</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <f t="shared" si="0"/>
         <v>0.46590909090909088</v>
       </c>
@@ -1851,7 +1865,7 @@
       <c r="F38">
         <v>31</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <f t="shared" si="0"/>
         <v>0.43867924528301894</v>
       </c>
@@ -1884,7 +1898,7 @@
       <c r="F39">
         <v>32.1</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <f t="shared" si="0"/>
         <v>0.46565774155995343</v>
       </c>
@@ -1917,7 +1931,7 @@
       <c r="F40">
         <v>30.5</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <f t="shared" si="0"/>
         <v>0.43414634146341463</v>
       </c>
@@ -1950,7 +1964,7 @@
       <c r="F41">
         <v>32.700000000000003</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <f t="shared" si="0"/>
         <v>0.45121951219512196</v>
       </c>
@@ -1983,7 +1997,7 @@
       <c r="F42">
         <v>34.700000000000003</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <f t="shared" si="0"/>
         <v>0.44831591173054591</v>
       </c>
@@ -2016,7 +2030,7 @@
       <c r="F43">
         <v>34.5</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <f t="shared" si="0"/>
         <v>0.47044917257683216</v>
       </c>
@@ -2049,7 +2063,7 @@
       <c r="F44">
         <v>32.6</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <f t="shared" si="0"/>
         <v>0.43020304568527917</v>
       </c>
@@ -2082,7 +2096,7 @@
       <c r="F45">
         <v>33.799999999999997</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="1">
         <f t="shared" si="0"/>
         <v>0.45627376425855509</v>
       </c>
@@ -2115,7 +2129,7 @@
       <c r="F46">
         <v>36.6</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="1">
         <f t="shared" si="0"/>
         <v>0.44988344988344992</v>
       </c>
@@ -2148,7 +2162,7 @@
       <c r="F47">
         <v>35.299999999999997</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
         <f t="shared" si="0"/>
         <v>0.45958429561200925</v>
       </c>
@@ -2181,7 +2195,7 @@
       <c r="F48">
         <v>25.4</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="1">
         <f t="shared" si="0"/>
         <v>0.47511312217194568</v>
       </c>
@@ -2214,7 +2228,7 @@
       <c r="F49">
         <v>25.7</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="1">
         <f t="shared" si="0"/>
         <v>0.47791619479048703</v>
       </c>
@@ -2247,7 +2261,7 @@
       <c r="F50">
         <v>33.1</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="1">
         <f t="shared" si="0"/>
         <v>0.44593088071348941</v>
       </c>
@@ -2280,7 +2294,7 @@
       <c r="F51">
         <v>32.299999999999997</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="1">
         <f t="shared" si="0"/>
         <v>0.45361990950226244</v>
       </c>
@@ -2313,7 +2327,7 @@
       <c r="F52">
         <v>26.5</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="1">
         <f t="shared" si="0"/>
         <v>0.45149253731343275</v>
       </c>
@@ -2346,7 +2360,7 @@
       <c r="F53">
         <v>25.5</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="1">
         <f t="shared" si="0"/>
         <v>0.48645161290322586</v>
       </c>
@@ -2379,7 +2393,7 @@
       <c r="F54">
         <v>31.2</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="1">
         <f t="shared" si="0"/>
         <v>0.46227544910179641</v>
       </c>
@@ -2412,7 +2426,7 @@
       <c r="F55">
         <v>29.4</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="1">
         <f t="shared" si="0"/>
         <v>0.46200241254523516</v>
       </c>
@@ -2445,7 +2459,7 @@
       <c r="F56">
         <v>33.299999999999997</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="1">
         <f t="shared" si="0"/>
         <v>0.46764346764346759</v>
       </c>
@@ -2478,7 +2492,7 @@
       <c r="F57">
         <v>32.6</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="1">
         <f t="shared" si="0"/>
         <v>0.48288075560802829</v>
       </c>
@@ -2511,7 +2525,7 @@
       <c r="F58">
         <v>29.1</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="1">
         <f t="shared" si="0"/>
         <v>0.4794841735052755</v>
       </c>
@@ -2544,7 +2558,7 @@
       <c r="F59">
         <v>28.3</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="1">
         <f t="shared" si="0"/>
         <v>0.48617511520737333</v>
       </c>
@@ -2577,7 +2591,7 @@
       <c r="F60">
         <v>34.1</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="1">
         <f t="shared" si="0"/>
         <v>0.45905420991926177</v>
       </c>
@@ -2610,7 +2624,7 @@
       <c r="F61">
         <v>31.8</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="1">
         <f t="shared" si="0"/>
         <v>0.47435897435897439</v>
       </c>
@@ -2628,39 +2642,39 @@
       <c r="A62" t="s">
         <v>36</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <f>AVERAGE(B2,B4,B6,B8,B10,B12,B14,B16,B18,B20,B22,B24,B26,B28,B30,B32,B34,B36,B38,B40,B42,B44,B46,B48,B50,B52,B54,B56,B58,B60)</f>
         <v>25.776666666666667</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <f>AVERAGE(C2,C4,C6,C8,C10,C12,C14,C16,C18,C20,C22,C24,C26,C28,C30,C32,C34,C36,C38,C40,C42,C44,C46,C48,C50,C52,C54,C56,C58,C60)</f>
         <v>18.463333333333335</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="2">
         <f>AVERAGE(D2,D4,D6,D8,D10,D12,D14,D16,D18,D20,D22,D24,D26,D28,D30,D32,D34,D36,D38,D40,D42,D44,D46,D48,D50,D52,D54,D56,D58,D60)</f>
         <v>4.2866666666666662</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <f>AVERAGE(E2,E4,E6,E8,E10,E12,E14,E16,E18,E20,E22,E24,E26,E28,E30,E32,E34,E36,E38,E40,E42,E44,E46,E48,E50,E52,E54,E56,E58,E60)</f>
         <v>6.6533333333333333</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2">
         <f>AVERAGE(F2,F4,F6,F8,F10,F12,F14,F16,F18,F20,F22,F24,F26,F28,F30,F32,F34,F36,F38,F40,F42,F44,F46,F48,F50,F52,F54,F56,F58,F60)</f>
         <v>31.583333333333336</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="2">
         <f t="shared" si="0"/>
         <v>0.45129224652087474</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="2">
         <f>AVERAGE(H2,H4,H6,H8,H10,H12,H14,H16,H18,H20,H22,H24,H26,H28,H30,H32,H34,H36,H38,H40,H42,H44,H46,H48,H50,H52,H54,H56,H58,H60)</f>
         <v>38.589999999999996</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="2">
         <f>AVERAGE(I2,I4,I6,I8,I10,I12,I14,I16,I18,I20,I22,I24,I26,I28,I30,I32,I34,I36,I38,I40,I42,I44,I46,I48,I50,I52,I54,I56,I58,I60)</f>
         <v>85.509999999999991</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="2">
         <f>AVERAGE(J2,J4,J6,J8,J10,J12,J14,J16,J18,J20,J22,J24,J26,J28,J30,J32,J34,J36,J38,J40,J42,J44,J46,J48,J50,J52,J54,J56,J58,J60)</f>
         <v>104.02</v>
       </c>
@@ -2669,51 +2683,41 @@
       <c r="A63" t="s">
         <v>67</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <f>AVERAGE(B61,B59,B57,B55,B53,B51,B49,B47,B45,B43,B41,B39,B37,B35,B33,B31,B29,B27,B25,B23,B21,B19,B17,B15,B13,B11,B9,B7,B5,B3)</f>
         <v>26.279999999999994</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="2">
         <f>AVERAGE(C3,C5,C7,C9,C11,C13,C15,C17,C19,C21,C23,C25,C27,C29,C31,C33,C35,C37,C39,C41,C43,C45,C47,C49,C51,C53,C55,C57,C59,C61)</f>
         <v>18.153333333333332</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="2">
         <f>AVERAGE(D3,D5,D7,D9,D11,D13,D15,D17,D19,D21,D23,D25,D27,D29,D31,D33,D35,D37,D39,D41,D43,D45,D47,D49,D51,D53,D55,D57,D59,D61)</f>
         <v>4.2100000000000009</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <f>AVERAGE(E3,E5,E7,E9,E11,E13,E15,E17,E19,E21,E23,E25,E27,E29,E31,E33,E35,E37,E39,E41,E43,E45,E47,E49,E51,E53,E55,E57,E59,E61)</f>
         <v>6.1766666666666667</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2">
         <f>AVERAGE(F61,F59,F57,F55,F53,F51,F49,F47,F45,F43,F41,F39,F37,F35,F33,F31,F29,F27,F25,F23,F21,F19,F17,F15,F13,F11,F9,F7,F5,F3)</f>
         <v>31.65666666666667</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="2">
         <f t="shared" si="0"/>
         <v>0.4778143565293072</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="2">
         <f>AVERAGE(H3,H5,H7,H9,H11,H13,H15,H17,H19,H21,H23,H25,H27,H29,H31,H33,H35,H37,H39,H41,H43,H45,H47,H49,H51,H53,H55,H57,H59,H61)</f>
         <v>39.460000000000008</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="2">
         <f>AVERAGE(I3,I5,I7,I9,I11,I13,I15,I17,I19,I21,,I23,I35,I27,I29,I31,I33,I35,I37,I39,I41,I43,I45,I47,I49,I51,I53,I55,I57,I59,I61,I25)</f>
         <v>82.584375000000009</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="2">
         <f>AVERAGE(J3,J5,J7,J9,J11,J13,J15,J17,J19,J21,J23,J25,J27,J29,J31,J33,J35,J37,J39,J41,J43,J45,J47,J49,J51,J53,J55,J57,J59,J61)</f>
         <v>107.17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64">
-        <f>AVERAGE(B2:B61)</f>
-        <v>26.028333333333332</v>
-      </c>
-      <c r="E64">
-        <f>AVERAGE(E2:E61)</f>
-        <v>6.415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>